<commit_message>
changement de l'espace de téléchargement
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/piratage/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95AF7EE-BB85-1B4F-BF78-6D5EC60B22A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9BBEC0-6DCF-D441-8F2B-84ABDDEDD964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="760" windowWidth="16360" windowHeight="17600" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -220,15 +220,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -237,10 +249,29 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -249,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,7 +288,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +608,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>45891.46875</v>
+        <v>45891.427083333336</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -626,8 +659,8 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
-        <v>45895.552083333336</v>
+      <c r="C3" s="4">
+        <v>45895.59375</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -644,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3">
-        <v>45898.46875</v>
+        <v>45898.427083333336</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -660,8 +693,8 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
-        <v>45902.552083333336</v>
+      <c r="C5" s="4">
+        <v>45902.59375</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -678,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>45905.46875</v>
+        <v>45905.427083333336</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
@@ -694,8 +727,8 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
-        <v>45912.552083333336</v>
+      <c r="C7" s="4">
+        <v>45912.59375</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -709,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3">
-        <v>45916.552083333336</v>
+        <v>45916.59375</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
@@ -725,8 +758,8 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <v>45919.46875</v>
+      <c r="C9" s="4">
+        <v>45919.427083333336</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
@@ -743,7 +776,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>45923.552083333336</v>
+        <v>45923.59375</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
@@ -759,8 +792,8 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
-        <v>45926.46875</v>
+      <c r="C11" s="4">
+        <v>45926.427083333336</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -777,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="3">
-        <v>45930.552083333336</v>
+        <v>45930.59375</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>44</v>
@@ -793,8 +826,8 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
-        <v>45933.46875</v>
+      <c r="C13" s="4">
+        <v>45933.427083333336</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>28</v>
@@ -811,7 +844,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>45937.552083333336</v>
+        <v>45937.59375</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -827,8 +860,8 @@
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="3">
-        <v>45940.46875</v>
+      <c r="C15" s="4">
+        <v>45940.427083333336</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -845,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="3">
-        <v>45951.552083333336</v>
+        <v>45951.59375</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -861,8 +894,8 @@
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="3">
-        <v>45954.46875</v>
+      <c r="C17" s="4">
+        <v>45954.427083333336</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -879,7 +912,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3">
-        <v>45958.552083333336</v>
+        <v>45958.59375</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>33</v>
@@ -895,8 +928,8 @@
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="3">
-        <v>45961.46875</v>
+      <c r="C19" s="4">
+        <v>45961.427083333336</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>34</v>
@@ -913,7 +946,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3">
-        <v>45965.552083333336</v>
+        <v>45965.59375</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
@@ -929,8 +962,8 @@
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="3">
-        <v>45968.46875</v>
+      <c r="C21" s="4">
+        <v>45968.427083333336</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>26</v>
@@ -947,7 +980,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="3">
-        <v>45972.552083333336</v>
+        <v>45972.59375</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>31</v>
@@ -963,8 +996,8 @@
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="3">
-        <v>45975.46875</v>
+      <c r="C23" s="4">
+        <v>45975.427083333336</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>38</v>
@@ -981,7 +1014,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="3">
-        <v>45979.552083333336</v>
+        <v>45979.59375</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>46</v>
@@ -997,8 +1030,8 @@
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="3">
-        <v>45982.46875</v>
+      <c r="C25" s="4">
+        <v>45982.427083333336</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
@@ -1012,7 +1045,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="3">
-        <v>45986.552083333336</v>
+        <v>45986.59375</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>48</v>
@@ -1028,8 +1061,8 @@
       <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="3">
-        <v>45989.46875</v>
+      <c r="C27" s="4">
+        <v>45989.427083333336</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>50</v>
@@ -1046,7 +1079,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="3">
-        <v>45993.552083333336</v>
+        <v>45993.59375</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>9</v>
@@ -1062,8 +1095,8 @@
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="3">
-        <v>45996.46875</v>
+      <c r="C29" s="4">
+        <v>45996.427083333336</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
@@ -1080,7 +1113,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="3">
-        <v>46000.552083333336</v>
+        <v>46000.59375</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
@@ -1096,8 +1129,8 @@
       <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="3">
-        <v>46003.46875</v>
+      <c r="C31" s="5">
+        <v>46003.427083333336</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
changement horaire - devancer hameçonnage
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/piratage/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E748359-2EE5-3F4E-8587-0406BBB57D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4145166B-A01D-3B47-A80E-14C330F11068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="760" windowWidth="16360" windowHeight="17600" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,10 +796,10 @@
         <v>45926.635416666664</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -813,7 +813,7 @@
         <v>45930.59375</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
@@ -830,7 +830,7 @@
         <v>45933.635416666664</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -847,7 +847,7 @@
         <v>45937.59375</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>37</v>
@@ -864,7 +864,7 @@
         <v>45940.635416666664</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -915,7 +915,7 @@
         <v>45958.59375</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
@@ -932,7 +932,7 @@
         <v>45961.635416666664</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>35</v>
@@ -949,7 +949,7 @@
         <v>45965.59375</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
@@ -966,7 +966,7 @@
         <v>45968.635416666664</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
         <v>27</v>
@@ -983,10 +983,10 @@
         <v>45972.59375</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">

</xml_diff>